<commit_message>
made all figures for design section. still have to discuss ankle design and experiments
</commit_message>
<xml_diff>
--- a/figures/winter_data_angle_torque.xlsx
+++ b/figures/winter_data_angle_torque.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitishthatte/Documents/OverleafDocs/thesis_proposal/figures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitishthatte/Documents/ResearchDocs/thesis_proposal/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Ankle angle (rad)</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Knee torque (N-m)</t>
+  </si>
+  <si>
+    <t>Ankle velocity</t>
   </si>
 </sst>
 </file>
@@ -353,21 +356,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="2" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,977 +378,1190 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-0.26529004630313807</v>
       </c>
       <c r="B2">
         <v>-1.6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
+        <v>-2.29</v>
+      </c>
+      <c r="D2">
         <v>0.81506876068135192</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>-7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-0.28623399732707</v>
       </c>
       <c r="B3">
         <v>-1.6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
+        <v>-0.82</v>
+      </c>
+      <c r="D3">
         <v>0.90931654028904574</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>-7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-0.28797932657906439</v>
       </c>
       <c r="B4">
         <v>-1.5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="D4">
         <v>0.99309234438477345</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>-6.9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-0.2722713633111154</v>
       </c>
       <c r="B5">
         <v>-1.3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D5">
         <v>1.064650843716541</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>-6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-0.24260076602721181</v>
       </c>
       <c r="B6">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
+        <v>2.34</v>
+      </c>
+      <c r="D6">
         <v>1.1187560505283651</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>-5.8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-0.20420352248333654</v>
       </c>
       <c r="B7">
         <v>-0.9</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
+        <v>2.78</v>
+      </c>
+      <c r="D7">
         <v>1.1554079648202462</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>-4.8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-0.16231562043547265</v>
       </c>
       <c r="B8">
         <v>-0.7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
+        <v>2.92</v>
+      </c>
+      <c r="D8">
         <v>1.1746065865921838</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>-3.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-0.12042771838760874</v>
       </c>
       <c r="B9">
         <v>-0.6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
+        <v>2.76</v>
+      </c>
+      <c r="D9">
         <v>1.1746065865921838</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-8.377580409572781E-2</v>
       </c>
       <c r="B10">
         <v>-0.5</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
+        <v>2.38</v>
+      </c>
+      <c r="D10">
         <v>1.1588986233242349</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-5.235987755982989E-2</v>
       </c>
       <c r="B11">
         <v>-0.4</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="D11">
         <v>1.1274826967883367</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-2.9670597283903602E-2</v>
       </c>
       <c r="B12">
         <v>-0.4</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
+        <v>1.41</v>
+      </c>
+      <c r="D12">
         <v>1.0821041362364843</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-1.2217304763960306E-2</v>
       </c>
       <c r="B13">
         <v>-0.5</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="D13">
         <v>1.0245082709206714</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>1.9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-1.7453292519943296E-3</v>
       </c>
       <c r="B14">
         <v>-0.5</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="D14">
         <v>0.95644043009289259</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>2.7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5.2359877559829881E-3</v>
       </c>
       <c r="B15">
         <v>-0.6</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D15">
         <v>0.87790061375314776</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>3.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1.0471975511965976E-2</v>
       </c>
       <c r="B16">
         <v>-0.6</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D16">
         <v>0.79237948040542561</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>4.2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1.2217304763960306E-2</v>
       </c>
       <c r="B17">
         <v>-0.6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="D17">
         <v>0.69987703004972612</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1.5707963267948967E-2</v>
       </c>
       <c r="B18">
         <v>-0.6</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D18">
         <v>0.60213859193804364</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>5.8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1.7453292519943295E-2</v>
       </c>
       <c r="B19">
         <v>-0.6</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D19">
         <v>0.50090949532237261</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>6.8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1.9198621771937627E-2</v>
       </c>
       <c r="B20">
         <v>-0.5</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D20">
         <v>0.39793506945470714</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2.2689280275926284E-2</v>
       </c>
       <c r="B21">
         <v>-0.3</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D21">
         <v>0.29496064358704166</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>9.4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2.7925268031909273E-2</v>
       </c>
       <c r="B22">
         <v>-0.1</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="D22">
         <v>0.2007128639793479</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>11.1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3.3161255787892259E-2</v>
       </c>
       <c r="B23">
         <v>0.1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D23">
         <v>0.11693705988362008</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>12.8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3.8397243543875255E-2</v>
       </c>
       <c r="B24">
         <v>0.3</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="D24">
         <v>4.7123889803846901E-2</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>14.3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4.3633231299858237E-2</v>
       </c>
       <c r="B25">
         <v>0.5</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="D25">
         <v>-1.7453292519943296E-3</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>15.1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4.3633231299858237E-2</v>
       </c>
       <c r="B26">
         <v>0.5</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
+        <v>-0.21</v>
+      </c>
+      <c r="D26">
         <v>-3.1415926535897934E-2</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>14.6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3.6651914291880923E-2</v>
       </c>
       <c r="B27">
         <v>0.5</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
+        <v>-0.79</v>
+      </c>
+      <c r="D27">
         <v>-4.014257279586958E-2</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>12.7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2.0943951023931952E-2</v>
       </c>
       <c r="B28">
         <v>0.3</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
+        <v>-1.54</v>
+      </c>
+      <c r="D28">
         <v>-3.1415926535897934E-2</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>9.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-6.9813170079773184E-3</v>
       </c>
       <c r="B29">
         <v>1.7</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
+        <v>-2.2400000000000002</v>
+      </c>
+      <c r="D29">
         <v>-1.0471975511965976E-2</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-4.3633231299858237E-2</v>
       </c>
       <c r="B30">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
+        <v>-2.63</v>
+      </c>
+      <c r="D30">
         <v>1.9198621771937627E-2</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>-8.2030474843733492E-2</v>
       </c>
       <c r="B31">
         <v>-8.3000000000000007</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
+        <v>-2.4700000000000002</v>
+      </c>
+      <c r="D31">
         <v>5.235987755982989E-2</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>7.6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>-0.11344640137963143</v>
       </c>
       <c r="B32">
         <v>-2.8</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
+        <v>-1.77</v>
+      </c>
+      <c r="D32">
         <v>8.9011791851710806E-2</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>4.5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>-0.13264502315156904</v>
       </c>
       <c r="B33">
         <v>-6.9</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
+        <v>-0.77</v>
+      </c>
+      <c r="D33">
         <v>0.1291543646475804</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>-7.8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>-0.1361356816555577</v>
       </c>
       <c r="B34">
         <v>-4.5999999999999996</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D34">
         <v>0.17104226669544431</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>-14.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>-0.12566370614359174</v>
       </c>
       <c r="B35">
         <v>-5</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="D35">
         <v>0.21118483949131386</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>-24.8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>-0.10471975511965978</v>
       </c>
       <c r="B36">
         <v>-2.6</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
+        <v>1.59</v>
+      </c>
+      <c r="D36">
         <v>0.24434609527920614</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>-31.6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>-8.028514559173916E-2</v>
       </c>
       <c r="B37">
         <v>0.5</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
+        <v>1.77</v>
+      </c>
+      <c r="D37">
         <v>0.26878070480712674</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>-35</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>-5.4105206811824215E-2</v>
       </c>
       <c r="B38">
         <v>-0.2</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
+        <v>1.71</v>
+      </c>
+      <c r="D38">
         <v>0.28274333882308139</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>-37.799999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>-3.1415926535897934E-2</v>
       </c>
       <c r="B39">
         <v>3.5</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
+        <v>1.52</v>
+      </c>
+      <c r="D39">
         <v>0.28448866807507572</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>-32.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>-1.0471975511965976E-2</v>
       </c>
       <c r="B40">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="D40">
         <v>0.2775073510670984</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>-28.1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>6.9813170079773184E-3</v>
       </c>
       <c r="B41">
         <v>6.6</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="D41">
         <v>0.26529004630313807</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>-24.8</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2.0943951023931952E-2</v>
       </c>
       <c r="B42">
         <v>10.5</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="D42">
         <v>0.24783675378319478</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <v>-20.2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3.6651914291880923E-2</v>
       </c>
       <c r="B43">
         <v>10.6</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="D43">
         <v>0.23038346126325149</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <v>-19.8</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>4.8869219055841226E-2</v>
       </c>
       <c r="B44">
         <v>14.1</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D44">
         <v>0.21467549799530256</v>
       </c>
-      <c r="D44" s="1">
+      <c r="E44" s="1">
         <v>-15.8</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5.9341194567807204E-2</v>
       </c>
       <c r="B45">
         <v>18.7</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="D45">
         <v>0.19896753472735357</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>-10.9</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>6.806784082777885E-2</v>
       </c>
       <c r="B46">
         <v>22.5</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="D46">
         <v>0.18675022996339324</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <v>-7.8</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>7.3303828583761846E-2</v>
       </c>
       <c r="B47">
         <v>25.3</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="D47">
         <v>0.17627825445142728</v>
       </c>
-      <c r="D47" s="1">
+      <c r="E47" s="1">
         <v>-6.6</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>8.028514559173916E-2</v>
       </c>
       <c r="B48">
         <v>27.9</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D48">
         <v>0.16406094968746698</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>-6.6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>8.5521133347722156E-2</v>
       </c>
       <c r="B49">
         <v>30.3</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="D49">
         <v>0.15358897417550102</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>-7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>9.250245035569947E-2</v>
       </c>
       <c r="B50">
         <v>33.5</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="D50">
         <v>0.143116998663535</v>
       </c>
-      <c r="D50" s="1">
+      <c r="E50" s="1">
         <v>-5.9</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>0.10297442586766545</v>
       </c>
       <c r="B51">
         <v>38.799999999999997</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="D51">
         <v>0.13264502315156904</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>0.11170107212763709</v>
       </c>
       <c r="B52">
         <v>45.1</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="D52">
         <v>0.12217304763960307</v>
       </c>
-      <c r="D52" s="1">
+      <c r="E52" s="1">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>0.11693705988362008</v>
       </c>
       <c r="B53">
         <v>45.4</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D53">
         <v>0.11170107212763709</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>0.12042771838760874</v>
       </c>
       <c r="B54">
         <v>53.5</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D54">
         <v>0.10297442586766545</v>
       </c>
-      <c r="D54" s="1">
+      <c r="E54" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>0.12042771838760874</v>
       </c>
       <c r="B55">
         <v>58.8</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="D55">
         <v>9.4247779607693802E-2</v>
       </c>
-      <c r="D55" s="1">
+      <c r="E55" s="1">
         <v>6.2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>0.12042771838760874</v>
       </c>
       <c r="B56">
         <v>64.8</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="1">
+        <v>-0.02</v>
+      </c>
+      <c r="D56">
         <v>9.0757121103705138E-2</v>
       </c>
-      <c r="D56" s="1">
+      <c r="E56" s="1">
         <v>7.9</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>0.11868238913561441</v>
       </c>
       <c r="B57">
         <v>71.2</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="D57">
         <v>8.9011791851710806E-2</v>
       </c>
-      <c r="D57" s="1">
+      <c r="E57" s="1">
         <v>10.4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>0.11868238913561441</v>
       </c>
       <c r="B58">
         <v>77.3</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="1">
+        <v>-0.05</v>
+      </c>
+      <c r="D58">
         <v>9.599310885968812E-2</v>
       </c>
-      <c r="D58" s="1">
+      <c r="E58" s="1">
         <v>12.5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>0.11868238913561441</v>
       </c>
       <c r="B59">
         <v>82.7</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="1">
+        <v>-0.22</v>
+      </c>
+      <c r="D59">
         <v>0.10821041362364843</v>
       </c>
-      <c r="D59" s="1">
+      <c r="E59" s="1">
         <v>12.4</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>0.11344640137963143</v>
       </c>
       <c r="B60">
         <v>87</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="1">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="D60">
         <v>0.12740903539558607</v>
       </c>
-      <c r="D60" s="1">
+      <c r="E60" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>0.10297442586766545</v>
       </c>
       <c r="B61">
         <v>89.7</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="1">
+        <v>-1.04</v>
+      </c>
+      <c r="D61">
         <v>0.15533430342749532</v>
       </c>
-      <c r="D61" s="1">
+      <c r="E61" s="1">
         <v>6.4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>8.377580409572781E-2</v>
       </c>
       <c r="B62">
         <v>89.8</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="1">
+        <v>-1.62</v>
+      </c>
+      <c r="D62">
         <v>0.19024088846738194</v>
       </c>
-      <c r="D62" s="1">
+      <c r="E62" s="1">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>5.5850536063818547E-2</v>
       </c>
       <c r="B63">
         <v>86.7</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="1">
+        <v>-2.21</v>
+      </c>
+      <c r="D63">
         <v>0.23212879051524585</v>
       </c>
-      <c r="D63" s="1">
+      <c r="E63" s="1">
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2.0943951023931952E-2</v>
       </c>
       <c r="B64">
         <v>79.7</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="1">
+        <v>-2.79</v>
+      </c>
+      <c r="D64">
         <v>0.28274333882308139</v>
       </c>
-      <c r="D64" s="1">
+      <c r="E64" s="1">
         <v>-6.5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>-2.4434609527920613E-2</v>
       </c>
       <c r="B65">
         <v>68.599999999999994</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="1">
+        <v>-3.4</v>
+      </c>
+      <c r="D65">
         <v>0.34208453339088862</v>
       </c>
-      <c r="D65" s="1">
+      <c r="E65" s="1">
         <v>-10.1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>-7.679448708775051E-2</v>
       </c>
       <c r="B66">
         <v>54.3</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="1">
+        <v>-4.03</v>
+      </c>
+      <c r="D66">
         <v>0.41015237421866746</v>
       </c>
-      <c r="D66" s="1">
+      <c r="E66" s="1">
         <v>-12.5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>-0.13962634015954636</v>
       </c>
       <c r="B67">
         <v>38.799999999999997</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="1">
+        <v>-4.5</v>
+      </c>
+      <c r="D67">
         <v>0.48520153205442362</v>
       </c>
-      <c r="D67" s="1">
+      <c r="E67" s="1">
         <v>-13.3</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-0.2059488517353309</v>
       </c>
       <c r="B68">
         <v>24.2</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="1">
+        <v>-4.54</v>
+      </c>
+      <c r="D68">
         <v>0.56548667764616278</v>
       </c>
-      <c r="D68" s="1">
+      <c r="E68" s="1">
         <v>-12.5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>-0.26878070480712674</v>
       </c>
       <c r="B69">
         <v>12.3</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="1">
+        <v>-3.97</v>
+      </c>
+      <c r="D69">
         <v>0.65275314024587927</v>
       </c>
-      <c r="D69" s="1">
+      <c r="E69" s="1">
         <v>-10.6</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>-0.31939525311496231</v>
       </c>
       <c r="B70">
         <v>3.6</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="1">
+        <v>-2.84</v>
+      </c>
+      <c r="D70">
         <v>0.74176493209759009</v>
       </c>
-      <c r="D70" s="1">
+      <c r="E70" s="1">
         <v>-6.8</v>
       </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C71" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>